<commit_message>
First version of new pipeline completed
</commit_message>
<xml_diff>
--- a/src/active_learning/agreement_es.xlsx
+++ b/src/active_learning/agreement_es.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,47 +462,47 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>416302</v>
+        <v>245962</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ES_1018513_128596-0</t>
+          <t>ES_88327_20401-0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Resúmenes: Los adultos de edad avanzada y mal alimentados, por lo general, presentan carencia de vitamina C, la cual puede conducir a una enfermedad nutricional como el escorbuto.</t>
+          <t>Lea sobre el valor de la exposición a diversas culturas para promover la equidad, la inclusión y el sentido de pertenencia.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>373465</v>
+        <v>462049</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EN_163691_46334-1</t>
+          <t>EN_22289_24687-47</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Kim Mook, MHS; Barbara A. Laraia, PhD; Vanessa M. Oddo, MPH; Jessica C. Jones-Smith, PhD: Suggested citation for this article: Mook K, Laraia BA, Oddo VM, Jones-Smith JC. Food Security Status and Barriers to Fruit and Vegetable Consumption in Two Economically Deprived Communities of Oakland, California, 2013–2014. Prev Chronic Dis 2016;13:150402. DOI: http://dx.doi.org/10.5888/pcd13.150402external icon.</t>
+          <t>OSHA [1998]. Profile of the wireless telecommunications industry and the telecommunications tower industry. (Contract No. J-9-F-4-0013, Jack Faucett Associates, Bethesda, Maryland.) Washington, DC: U.S. Department of Labor, Occupational Safety and Health Administration.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -518,215 +518,215 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>423650</v>
+        <v>1032285</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>EN_90546_38611-151</t>
+          <t>ES_987172_127047-1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Reducing the environmental impact from the manufacture and use of products.</t>
+          <t>Con el tiempo, las personas que tienen diabetes y niveles altos de azúcar en la sangre pueden desarrollar complicaciones graves o que ponen en riesgo la vida, incluyendo enfermedad cardíaca, accidente cerebrovascular, problemas renales, daño a los nervios y problemas de la visión. Usar medicamentos, hacer cambios en el estilo de vida (por ejemplo, en la dieta, ejercitarse, dejar de fumar), y controlar regularmente su nivel de azúcar en la sangre puede ayudarle a controlar su diabetes y a mejorar su salud. Esta terapia también puede reducir las posibilidades de sufrir un ataque cardíaco, accidente cerebrovascular u otras complicaciones relacionadas con la diabetes como insuficiencia renal, daño a los nervios (entumecimiento, piernas o pies fríos, problemas de función sexual en hombres y mujeres), problemas de visión, incluyendo daños o pérdida de la vista, o enfermedad de las encías. Su médico y otros proveedores de atención médica hablarán con usted sobre cómo manejar mejor su diabetes.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>940775</v>
+        <v>481456</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EN_812443_119576-52</t>
+          <t>ES_370662_44971-8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Reviewed on Sep 15, 2022: Excellent experience with Dr. Kaiser and his staff.</t>
+          <t>Cada año, Asistencia Jurídica en el Trabajo recibe noticias de demasiados trabajadores que se han visto obligados a elegir entre estar al lado de sus familias o conservar su empleo. Un padre primerizo, cuyo empleador era demasiado pequeño para estar cubierto por las actuales leyes de protección del empleo, fue despedido de su trabajo de camarero cuando se tomó dos semanas para establecer un vínculo afectivo con su bebé, que nació con complicaciones de salud.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[0, 1, 0, 1]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[0, 1, 0, 1]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>127209</v>
+        <v>948398</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EN_355790_55488-1</t>
+          <t>ES_1057085_9955-2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Background: Cigarette smoking remains the leading cause of preventable morbidity and mortality in the United States. Despite overall declines in cigarette smoking, a high prevalence of smoking persists among certain subpopulations, including persons with mental illness.</t>
+          <t>El género Manfreda pertenece a la familia Asparagaceae, subfamilia Agavoideae (APG III, 2009). Se distribuye desde el sureste de los EUA, hasta el norte de Nicaragua. México es el centro de diversidad del género. De las 32 especies reconocidas, 31 (97%) son propias de este país (Castillejos, 2009), la mayoría consideradas como microendemismos, debido a que ocupan menos del 1.5% del territorio nacional (García-Mendoza, 1995).</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>940740</v>
+        <v>622180</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EN_1214355_278532-2</t>
+          <t>ES_893691_118877-14</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>There are several tests for color vision. During the most common, you will be shown several cards with colored dot patterns. These cards are called Ishihara plates. In the patterns, some of the dots will appear to form numbers or symbols. You will be asked to identify the symbols, if possible.</t>
+          <t>El siguiente informe de caso es un ejemplo de los diversos riesgos que enfrentan los jinetes en la industria hípica durante su trabajo. NIOSH realizó la investigación de este caso mediante su Programa de análisis de tasas de mortalidad y evaluación de control [NIOSH 2007b].</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>957893</v>
+        <v>599881</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EN_98878_39921-1</t>
+          <t>ES_11560_992-26</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Learn more about how Candida develops antimicrobial resistance and causes illness.</t>
+          <t>Espacio: Describir cómo tu empresa proporcionará áreas privadas donde las mujeres podrán extraerse leche. La política puede especificar:</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>940750</v>
+        <v>756942</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>EN_62503_33613-2</t>
+          <t>EN_580457_94921-17</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>NIOSH investigators offer the following recommendations to address general safety and health issues. It is possible that if some of the recommended programs had been in place, the LT’s death may have been prevented.</t>
+          <t>Kost S. Pinworms. IN: Fleisher &amp; Ludwig’s 5-Minute Pediatric Emergency Medicine Consult, Hoffman RJ, Wang VJ, and Scarfone RJ, eds. Wolters Kluwer/Lippincott Williams &amp; Wilkins, Philadelphia, 2012.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>301902</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ES_490955_64059-16</t>
+          <t>ES_782199_102555-45</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Cada vez está más claro, en especial en el caso de los meduloblastomas, que el desenlace también se relaciona con las características moleculares del tumor; sin embargo, esto no se ha demostrado de forma definitiva en el caso de otros tumores embrionarios.[1,5,6,19-21] Las tasas de SG oscilan entre el 40 % y el 90 %, según el subtipo molecular de meduloblastoma y, posiblemente, según otros factores como el grado de diseminación en el momento del diagnóstico y el alcance de la resección. Los niños con meduloblastoma que sobreviven durante 5 años se consideran curados de su tumor. Por lo general, las tasas de supervivencia para otros tumores son más precarias y oscilan entre el 5 % y el 50 %. Las tasas de supervivencia específicas se tratan en cada subgrupo en este resumen.[22-25]</t>
+          <t>Antes de quedar embarazada, debería analizar la posibilidad de buscar asesoramiento previo a la concepción. Un especialista con experiencia en el embarazo y las enfermedades del corazón puede ayudarla.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[1, 0, 1, 0]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[1, 0, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>501839</v>
+        <v>177826</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>EN_752161_113736-11</t>
+          <t>ES_1016720_128264-10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Retainers: If you wear braces or clear aligners, you’ll need a retainer once your orthodontic treatment ends. A retainer is a custom oral appliance that keeps your teeth from drifting out of their proper positions. Your orthodontist can tell you how often you’ll need to wear your retainer to maintain the results of treatment.</t>
+          <t>Los rangos de los valores normales pueden variar ligeramente entre diferentes laboratorios. Hable con su médico sobre el significado de los resultados específicos de su examen.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -742,47 +742,47 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>547113</v>
+        <v>329263</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ES_777012_102025-1</t>
+          <t>ES_371282_45277-0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>¿De qué se trata esta prueba: Es un análisis de sangre para medir los niveles de proteínas que tiene en el cuerpo. El hígado produce la mayor parte de las proteínas que hay en la sangre. La albúmina es uno de los principales tipos de proteínas. La albúmina transporta por todo el organismo muchas otras sustancias, entre ellas medicamentos y elementos que produce el cuerpo. Otro tipo de proteína, llamada globulina, tiene otras funciones en el cuerpo.</t>
+          <t>Katherine Wutchiett explica cómo tomarse un permiso familiar y qué hacer al volver al trabajoLeer artículo de prensa: https://laist.com/news/education/early-childhood-education-pre-k/how-to-take-family-leave-california-rights-when-back-to-work</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>827653</v>
+        <v>824304</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ES_162581_37642-38</t>
+          <t>EN_760145_114414-21</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>La bulimia entre los adolescentes con diabetes tipo 1 se está haciendo cada vez más común. Estos adolescentes a menudo bajan de peso antes de que su diabetes sea descubierta, luego aumentan rápidamente de peso cuando comienza el tratamiento. Algunos aprenden que pueden bajar de peso saltándose las dosis de insulina. Esto causa un control deficiente de su diabetes y puede provocar problemas graves que pueden ocasionar ceguera o insuficiencia renal.</t>
+          <t>What’s the prognosis (outlook) for people with pulled calf muscles: Most people recover fully from pulled calf muscles without any permanent damage. Ask your healthcare provider when you can gradually start to do light activities again. Depending on the severity of your injury, it may be several weeks before you can return to full activities.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -798,47 +798,47 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>709210</v>
+        <v>239811</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>EN_665107_14531-44</t>
+          <t>ES_892721_118789-27</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Nanjala Madina is an HIV-positive mother of 10 children who makes a living selling vegetables along the streets of her working-class neighborhood in Kampala. She learned her HIV positive status in 2002 when health workers from Reach Out Mbuya Parish HIV/AIDS Initiative (ROM) came to her neighborhood for community HIV sensitization. “I had four children then,” she recalls.</t>
+          <t>El módulo “Silicosis: Guía de la industria para la concientización y prevención” (Silicosis – An Industry Guide to Awareness and Prevention) del Instituto Estadounidense del Mármol (MIA, por sus siglas en inglés) ofrece consejos para controlar la exposición a sílice durante las operaciones de corte de piedras. Está disponible para trabajadores y empleadores en el sitio web del MIA: www.marble-institute.com/silica/Silicosis_Industry_Guide_Tech_Module_2008.pdfpdf iconexternal icon. Se pueden encontrar otros recursos del MIA en www.marble-institute.com/silicaexternal icon.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[1, 1, 1, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[1, 1, 1, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>591216</v>
+        <v>1043191</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>EN_70857_34459-7</t>
+          <t>ES_809675_104364-4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>On the afternoon before the incident, the farm worker (victim #1) and a co-worker went to the manure pit to pump it out, but found that the pump intake was clogged with debris. The men tried to raise the pump from the pit but the 3-inch wire rope attached to the eye bolt at the top of the pump broke. The two men then decided to wait until the following morning to repair the pump and replace the wire rope.</t>
+          <t>El término actividades terroristas cubre varias acciones típicamente asociadas con el terrorismo, tal como el secuestro de personas; asesinatos; secuestro de aviones; agentes nucleares, biológicos, o químicos; uso de armas de fuego u otros artefactos peligrosos, entre otros.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -854,47 +854,47 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>1027604</v>
+        <v>360482</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ES_206852_38425-8</t>
+          <t>ES_478868_63328-3</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Durante la primera visita de una persona al dentista, se suele tomar una serie de radiografías periapicales de toda la boca (alrededor de 14 a 21 radiografías). Las radiografías de mordida se utilizan durante los chequeos para detectar caries dentales. Las radiografías panorámicas se pueden utilizar de vez en cuando. Las radiografías dentales se programan cuando sean necesarias, en base a la edad, el riesgo de enfermedades y las señales de enfermedad.</t>
+          <t>Accessed June 18, 2019. Benetti C, et al. Course of acute nonspecific mesenteric lymphadenitis: Single-center experience. European Journal of Pediatrics. 2018;177:243. Ferri FF. Mesenteric adenitis. In: Ferri's Clinical Advisor 2020. Philadelphia, Pa.: Elsevier; 2019. https://www.clinicalkey.com. Accessed June 19, 2019. AAP Committee on Infectious Diseases. Recommendations for prevention and control of influenza in children, 2017-2018. Pediatrics. 2017;140:e20172550. Sullivan JE, et al. Clinical report — Fever and antipyretic use in children. Pediatrics. 2011;127:580. Reaffirmed July 2016. 201.314 labeling of drug preparations containing salicylates. Electronic Code of Federal Regulations. https://www.ecfr.gov/cgi-bin/text-idx?SID=76be002fc0488562bf61609b21a6b11e&amp;mc=true&amp;node=se21.4.201_1314&amp;rgn=div8. Accessed Feb. 22, 2018. Renaud DL (expert opinion). Mayo Clinic, Rochester, Minn. Feb. 27, 2018. Relacionado Procedimientos asociados Ecografía abdominal Productos y servicios Boletín informativo: Mayo Clinic Health Letter — Edición digital Mayo Clinic Family Health Book (Libro de Mayo Clinic sobre la salud familiar), 5.ª edición Mostrar más productos y servicios de Mayo Clinic Linfadenitis mesentéricaSíntomasycausasDiagnósticoytratamiento Advertisement Mayo Clinic no respalda compañías ni productos. Las recaudaciones de los avisos comerciales financian nuestra misión sin fines de lucro. Avisos comerciales y patrocinio Política Oportunidades Opciones de avisos Prensa de Mayo Clinic Consulta estos éxitos de venta y ofertas especiales en libros y boletines informativos de Mayo Clinic Press.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>220415</v>
+        <v>74908</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ES_1052939_9775-14</t>
+          <t>EN_496688_10908-2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>De acuerdo con el pensador austríaco, entonces, la sociología comprensiva debe sustentarse en una teoría rigurosa del modo en que los sujetos pre-científicos experimentan, conocen e interpretan su Lebenswelt. Como es sabido, Schutz encuentra atisbos de una teoría tal en la fenomenología de Edmund Husserl; una posición filosófica que se esfuerza por rehabilitar el estatus de la experiencia vivida en primera persona, la cual fue sistemáticamente olvidada y descuidada en la Modernidad por diferentes tipos de reduccionismo: el naturalismo, el historicismo y el psicologismo (Waldenfels, 2009: 269).</t>
+          <t>Self-guided visits are available for groups of up to 50 people. Reservations are required for groups with more than 10 people.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -910,19 +910,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>296116</v>
+        <v>1044235</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ES_890730_118652-63</t>
+          <t>ES_1053814_9797-90</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5. Establecer programas de bloqueo e identificación con etiquetas que requieran candados y llaves asignados individualmente para asegurar los dispositivos de control de energía: Los programas de bloqueo e identificación con etiquetas deben sustentarse en el principio de únicamente una llave por cada candado controlado por el trabajador.** Esto significa lo siguiente:</t>
+          <t>Para Walsh, la interculturalidad que promueve el Estado ecuatoriano se ha vuelto «funcional», pues sirve a un «proyecto modernizador» (Walsh, 2014). En cambio, la uinpi-aw se identificaba con una «interculturalidad crítica», que quiso ser también una «práctica política» (Walsh, 2010: 89), es decir, una práctica decolonizadora. Según resume Walsh, todavía no existe, «es algo por construir» (Walsh, 2010: 78). En ese sentido, la no acreditación y el cierre de la uinpi-aw no ha significado el fin de esa institución académica, sino solamente una nueva etapa, pues las autoridades de la uinpi-aw decidieron que el proceso renazca fuera de los patrones formales de la educación institucionalizada. Pocas semanas después de la decisión del ceaaces de cerrar la Universidad, por no cumplir con estándares de calidad para su acreditación, se creó la Organización Comunitaria Pluriversidad Amawtay Wasi, que fue reconocida legalmente por el Consejo de Desarrollo de las Nacionalidades y Pueblos del Ecuador (codenpe) en los primeros días de diciembre de 2013 (codenpe, 2013).</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -938,75 +938,75 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>946307</v>
+        <v>106105</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>EN_1205015_277367-8</t>
+          <t>ES_435276_55804-2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>What happens during a Legionella test: Legionella tests may be done in urine, sputum, or blood.</t>
+          <t>Mostrando 1-1 de 1 médicos disponibles Inicial del apellido: E Kunle I. Elegbede, M.D., Ph.D. cirujano plástico Jacksonville, FL Áreas de especialización: Reconstrucción de los senos, reconstrucción microvascular , Abdominoplastia, Aumento de senos, Cirugía estética, Recons...trucción de los senos con cirugía de colgajo, Reconstrucción de los senos con implantes , injerto de nervio periférico, cirugía oncoplástica conservadora de mamas, Cirugía microvascular, baipás linfovenoso, Cirugía reconstructiva, Linfedema, linfedema por cáncer de mama Mostrar más áreas de especialización para Kunle I. Elegbede, M.D., Ph.D. Solicite una consulta Enfermedades tratadasGrupos especializados Nov. 14, 2020 Comparte en: FacebookTwitter Cirugía plástica y reconstructivaSeccionesPanorama generalSolicita una consultaAnálisis y procedimientosEnfermedades tratadasMédicosGrupos especializadosCentros, viajes y alojamientoEnsayos clínicosInvestigaciónCostos y seguroNoticias de Mayo ClinicRemisiones SeccionesSolicita una consultaPanorama generalAnálisis y procedimientosEnfermedades tratadasMédicosGrupos especializadosCentros, viajes y alojamientoEnsayos clínicosInvestigaciónCostos y seguroNoticias de Mayo ClinicRemisiones ORG-20473034 Centros y departamentos médicos Cirugía plástica y reconstructiva</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>297603</v>
+        <v>359014</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>EN_373225_57310-7</t>
+          <t>ES_49257_12702-3</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Lara M, Akinbami L, Flores G, Morgenstern H. Heterogeneity of childhood asthma among Hispanic children: Puerto Rican children bear a disproportionate burden. Pediatrics 2006;117:43--53.</t>
+          <t>Utilice los cinco pasos del método científico para ayudar a ampliar la comprensión de los niños sobre su entorno.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[0, 1, 0, 0]</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[0, 1, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>617918</v>
+        <v>730246</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>EN_45807_30875-39</t>
+          <t>ES_94997_22083-0</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Our subject matter experts hope to share some solutions that will be translatable to all of you in your individual laboratories. We also hope you will participate in the discussion by sharing your knowledge and experience.</t>
+          <t>Use esta hoja de trabajo electrónica para calcular el salario no gastado y el dinero de los beneficios complementarios relacionados con la falta de personal y para tomar decisiones sobre cómo volver a presupuestar esos fondos.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1022,75 +1022,75 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>319000</v>
+        <v>1051811</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ES_274571_40335-0</t>
+          <t>ES_84632_19485-0</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>¿Es para usted este tema: Este tema proporciona información sobre el asma en los niños. Si está buscando información sobre el asma en adolescentes y adultos, vea el tema Asma en adolescentes y adultos.</t>
+          <t>Analice los factores que causan caries y los factores que protegen los dientes de la caries dental. Descubra por qué es importante equilibrar estos factores y compartir esta información con los padres.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>1169607</v>
+        <v>849413</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>EN_159028_46168-8</t>
+          <t>ES_436793_56736-2</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Increasing people’s awareness of how they actually use time and messages targeting screen time are promising.</t>
+          <t>Mostrando 1-2 de 2 médicos disponibles Inicial del apellido: B Uldis Bite, M.D. cirujano plástico cirujano plástico facial Rochester, MN Áreas de especialización: cirugía craneofacial, Rinoplastia, Blefaroplastia, Cirugía para levantamiento de cejas, Cirugía estética en la cara, Ci...rugía estética, reconstrucción facial , cirugía de feminización facial, Implantación craneofacial, Reparación del labio leporino, Reparación del paladar hendido, Transferencia de tejido adiposo, Reparación de fractura facial, Parálisis de Bell, Craneosinostosis, Fisura del paladar , lesión facial, Fractura orbital, deformidad facial, Labio leporino Mostrar más áreas de especialización para Uldis Bite, M.D. Elizabeth A. Bradley, M.D. oftalmólogo Rochester, MN Áreas de especialización: Blefaroplastia, Cirugía de reanimación facial, Cuidado de los ojos, cirugía de descompresión orbitaria, reparación de p...tosis palpebral, reconstrucción orbitaria, Cirugía reconstructiva, dacriocistorrinostomía, biopsia, Ptosis de párpado, Enfermedad de Graves, cáncer de piel facial, Tumores y masas, deformidad facial, trastorno del nervio facial, Problema en el ojo Mostrar más áreas de especialización para Elizabeth A. Bradley, M.D. Solicite una consulta Enfermedades tratadasMédicos por especialidad Nov. 11, 2023 Comparte en: FacebookTwitter Centro de Medicina &amp; Cirugía Estética en RochesterSeccionesSolicita una consultaPanorama generalCirugía de mamasTratamientos corporalesTratamientos facialesTratamientos en la pielAnálisis y procedimientosEnfermedades tratadasMédicosMédicos por especialidadCentros, viajes y alojamientoInvestigaciónCostos y seguroRemisiones SeccionesSolicita una consultaPanorama generalCirugía de mamasTratamientos corporalesTratamientos facialesTratamientos en la pielAnálisis y procedimientosEnfermedades tratadasMédicosMédicos por especialidadCentros, viajes y alojamientoInvestigaciónCostos y seguroRemisiones ORG-20519186 Centros y departamentos médicos Centro de Medicina &amp; Cirugía Estética en Rochester</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>400571</v>
+        <v>557502</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ES_25291_10623-48</t>
+          <t>ES_47669_12479-21</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>El Servicio de Patología Forense del IMLCFCM tiene asignadas, entre sus funciones, la práctica de las autopsias en los casos de muerte violenta y sospechosa de criminalidad y la identificación de cadáveres.</t>
+          <t>¡Ordene los materiales de YMYG para su programa: Si bien se puede acceder a todas las herramientas de YMYG en línea, los programas pueden solicitar copias impresas de varias publicaciones diferentes que ofrece la CFPB, todo de forma gratuita. Solicite copias del kit de herramientas de YMYG (en inglés y español), Folletos para facilitar las conversaciones sobre el dinero (en inglés) y Guías complementarias (en inglés) para comunidades militares, comunidades indígenas, personas con discapacidades y personas con antecedentes penales.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1106,215 +1106,215 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>896207</v>
+        <v>655234</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ES_357864_43512-5</t>
+          <t>EN_592167_96880-49</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Las ronchas o habones rojos aparecen cuando los mastocitos del torrente sanguíneo segregan una sustancia química llamada "histamina", que hace que los diminutos vasos sanguíneos que hay debajo de la piel tengan escapes. El líquido se acumula dentro de la piel y forma granos y/o habones de gran tamaño. Esto puede ocurrir por varias razones. Pero, en muchos casos, no se llega a identificar la causa.</t>
+          <t>2022: Mark G. Evans, Jason Saliba, Yassmine Akkari, Deepa Bhojwani, Piers Blombery, Arpad Danos, Paul G. Ekert, Mark D. Ewalt, Sandeep Gurbuxani, Christine J. Harrison, Ilaria Iacobucci, Shai Izraeli, Nitin Jain, Rashmi Kanagal-Shamanna, Chimène Kesserwan, Alexandra E. Kovach, Kristy Lee, Hannah Helber, Valentina Nardi, Shalini Reshmi, Kathryn Roberts, Alexandre Rouette, Neerav Shukla, Wendy Stock, Panieh Terraf, Xinjie Xu, Liying Zhang, Xiaonan Zhao, Yiming Zhong, Gordana Raca, Obi L. Griffith, Malachi Griffith, Kilannin Krysiak, Charles Mullighan: Variant Curation of BCR::ABL1-like B-lymphoblastic leukemia/lymphoma Through Expert Panel Consensus. Cancer Genomics Consortium Annual Meeting 2022.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>970413</v>
+        <v>640928</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ES_504432_5906-1</t>
+          <t>EN_591078_96846-0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>En noviembre de 2020, el Programa Reconstruir celebró la finalización de las mejoras hechas en el sitio por un valor de USD 1 100 000.</t>
+          <t>Background: Lisa Guay-Woodford, MD, is Senior Advisor for Clinical and Translational Research Initiatives and an attending physician at Children’s Hospital of Philadelphia in the Divisions of Nephrology and Human Genetics. She is a professor of Pediatrics in the Perelman School of Medicine at the University of Pennsylvania. Dr. Guay-Woodford will direct a newly created Inherited Renal Diseases Program, which will span the Division of Nephrology and the Division of Human Genetics.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B27" t="n">
-        <v>628753</v>
+        <v>85859</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ES_224481_38889-57</t>
+          <t>ES_370159_44912-0</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Apoyo para la familia: Cuando una persona tiene ataques de pánico, toda su familia se ve afectada.</t>
+          <t>El gobernador Jerry Brown ha firmado el proyecto de ley SB 579, cuya autora es la senadora estatal Hannah-Beth Jackson (demócrata de Santa Bárbara), que amplía las protecciones laborales a los padres que se toman una excedencia por emergencias en el cuidado de los hijos o por visitas para evaluar o matricular a sus hijos en una escuela o guardería.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[0, 1, 1, 1]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[0, 1, 1, 1]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="B28" t="n">
-        <v>785517</v>
+        <v>652954</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>EN_436757_64030-7</t>
+          <t>EN_955447_165027-4</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>One of the national health objectives for the year 2000 is to eliminate occupational lead exposures that result in workers having blood lead concentrations greater than 25 ug/dL (objective 10.8) (2). Both the Council of State and Territorial Epidemiologists and the American Medical Association have endorsed positions encouraging health departments to make elevated BLLs in children and adults a notifiable condition nationwide.</t>
+          <t>Some kids can hold back their tics for a short time. But as tension builds, eventually it must be released as a tic. And if a person is concentrating on controlling the tic, it may be hard to focus on anything else. This can make it hard for kids with Tourette syndrome to have a conversation or pay attention in class.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 1]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 1]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="B29" t="n">
-        <v>406118</v>
+        <v>940735</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ES_415888_50936-14</t>
+          <t>EN_410845_61855-14</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Te sientas quieta durante 10 minutos mientras las cámaras gamma registran una imagen. Se pueden colocar almohadas detrás de la espalda para que estés más cómoda. Las almohadas ayudan a mantenerte en su lugar para que puedas relajarte durante la prueba. Deberías respirar de manera natural.</t>
+          <t>Louis Harris and Associates, Inc. `Public health': two words few people understand even though almost everyone thinks public health functions are very important. New York: Louis Harris and Associates, Inc., 1997.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="B30" t="n">
-        <v>492944</v>
+        <v>853674</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>EN_665419_14593-26</t>
+          <t>ES_66222_15339-0</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>When she first disclosed her HIV status, she was kicked out of her church, scorned by her neighbors and abandoned by her partner. But today, she and her sons have built a new home near the center of this rural community. She appears in newspapers and on the radio touting the importance of HIV testing and treatment and of self-acceptance and is seen as one of the region’s foremost HIV advocates.</t>
+          <t>La comunicación es una parte extremadamente importante de su plan de emergencias, y por lo general se pasa por alto en la fase de preparación. Utilice la hoja de trabajo Establecer sus procedimientos de comunicación (hoja de trabajo) para planificar cómo usted y el personal interactuarán entre ustedes, con los socorristas, los niños y las familias durante una emergencia.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[1, 0, 1, 1]</t>
+          <t>[0, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[1, 0, 1, 1]</t>
+          <t>[0, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>761586</v>
+        <v>598114</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ES_431708_54925-1</t>
+          <t>ES_678599_95478-0</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Para buscar una afección que comienza con la letra P P Para buscar una afección que comienza con la letra Q Q Para buscar una afección que comienza con la letra R R Para buscar una afección que comienza con la letra S S activo Para buscar una afección que comienza con la letra T T No hay ninguna afección que comience con la letra U U Para buscar una afección que comienza con la letra V V No hay ninguna afección que comience con la letra W W No hay ninguna afección que comience con la letra X X No hay ninguna afección que comience con la letra Y Y No hay ninguna afección que comience con la letra Z Z ES-View All ES-View All ES-View All Telangiectasia hemorrágica hereditaria Trastorno metabólico Trastornos genéticos Trastornos intestinales funcionales Trastornos metabólicos hereditarios Trastornos quísticos Tumor del estroma gastrointestinal Tumor neuroendocrino de colon Tumor neuroendocrino rectal Tumores carcinoides Tumores neuroendocrinos Tumores neuroendocrinos pancreáticos Solicite una consulta Análisis y procedimientosMédicos Feb. 06, 2024 Comparte en: FacebookTwitter Mayo Clinic de Rochester, Minnesota, ha sido reconocida como el mejor hospital de gastroenterología y cirugía gastrointestinal del país durante el período 2023-2024 por U.S. News &amp;amp; World Report. Obtén más información sobre este gran honor Gastroenterología y HepatologíaPágina inicialdel departamentoSeccionesSolicita una consultaPanorama generalAnálisis y procedimientosEnfermedades tratadasMédicosMédicos por sede y especialidadGrupos por especialidadConocimientos y categoríasCentros, viajes y alojamientoEnsayos clínicosInvestigaciónHistorias de pacientesCostos y seguroNoticias de Mayo ClinicRemisiones SeccionesSolicita una consultaPanorama generalMédicos por sede y especialidadGrupos por especialidadConocimientos y categoríasCentros, viajes y alojamientoInvestigaciónCostos y seguroRemisiones ORG-20308333 Centros y departamentos médicos Gastroenterología y Hepatología</t>
+          <t>El aborto en casa (mediante una cita de telesalud por video) te permite recibir un cuidado compasivo y experto para el aborto en la comodidad de tu propio hogar, en lugar de un centro de salud. Esta puede ser una buena opción si el transporte, el cuidado infantil o el tiempo libre del trabajo te dificultan programar una cita para hacer este proceso en uno de nuestros centros de salud.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>756168</v>
+        <v>120121</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ES_524652_64574-50</t>
+          <t>ES_568811_66300-13</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>El linfoma folicular in situ y el linfoma folicular primario de duodeno son variantes de crecimiento lento que con poca frecuencia progresan o requieren tratamiento.[33,34] El linfoma folicular ganglionar de tipo pediátrico tiene un comportamiento de crecimiento lento y rara vez recidiva; los pacientes adultos con esta variante histológica se caracterizan por una falta de reordenamiento de BCL2 junto con un índice de proliferación de Ki-67 superior al 30 % y una presentación localizada en estadio I.[35]</t>
+          <t>Los beneficios del entrenamiento de fuerza aumentan a medida que envejeces, dice Fielding. Mantener la fuerza es esencial para un envejecimiento saludable.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1330,103 +1330,103 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="B33" t="n">
-        <v>708739</v>
+        <v>446704</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ES_750223_100468-1</t>
+          <t>ES_785761_102791-1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Además del encéfalo y la médula espinal, los órganos principales del sistema nervioso son:</t>
+          <t>Las Condiciones Investigadas por los Programas de La Medicina del Medio Ambiente</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B34" t="n">
-        <v>785560</v>
+        <v>1299448</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>EN_968101_166232-9</t>
+          <t>EN_478716_70210-2</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>For other items not accepted, contact your local or county waste service or recycling service.</t>
+          <t>The itching may go on for many weeks after the initial treatment of the scabies. If scabies is still present after this time, or if new burrows appear, call your child’s healthcare provider. Your child may need to be retreated.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="B35" t="n">
-        <v>940829</v>
+        <v>71138</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>EN_128051_43798-17</t>
+          <t>ES_83325_19183-1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>* All plenary sessions will be webcast by the Kaisernetwork.org, a free service of the Kaiser Family Foundation. The webcast and transcript will be available at www.kaisernetwork.org/healthcast/phl/jun02.</t>
+          <t>Los recursos a continuación se centran en bebidas saludables, como agua, leche y jugo de frutas o verduras, y su importancia para mantener una buena salud oral, nutrición y salud en general. Estos recursos llaman la atención sobre los riesgos asociados con las bebidas que contienen azúcar agregada, como refrescos /sodas, bebidas de frutas y bebidas energéticas. También destacan cómo las bebidas poco saludables pueden contribuir a la caries dental, la diabetes y la obesidad en los niños pequeños. Vea también recursos sobre alimentación saludable.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="B36" t="n">
-        <v>785505</v>
+        <v>591145</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>EN_349654_54837-4</t>
+          <t>ES_244542_39476-4</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>To estimate the seroprevalence of infection with SARS-CoV-2 in Oregon, a cross-sectional, population-based convenience sample for SARS-CoV-2 immunoglobulin G (IgG) antibody testing was collected from mid-May through mid-June, in alignment with the World Health Organization seroepidemiologic investigation protocol.† Eighty-six facilities participating in CDC’s Influenza-like Illness Surveillance Network§ and Oregon’s Electronic Surveillance System for the Early Notification of Community-based Epidemics¶ were randomized and approached sequentially with a goal of recruiting 18 facilities to provide 50 specimens each. Facilities were asked to submit random subsamples of deidentified sera from patients of all ages visiting any ambulatory, emergency, or inpatient health care setting and to include the specimen collection date and the patient’s date of birth. Specimens were stored according to instructions provided by the test manufacturer and transported to the Oregon State Public Health Laboratory for testing with the Abbott Architect Laboratories SARS-CoV-2 IgG immunoassay. Abbott Laboratories (Abbott Park, Illinois) reports a sensitivity of 96.8% at ≥14 days after a positive polymerase chain reaction test result and specificity of 99.1%–100% (1). Results from actual use support the reported analytical performance of this test (2).</t>
+          <t>¿Qué causa el melanoma: Usted puede tener melanoma por pasar demasiado tiempo al sol. Demasiada radiación UV por exposición al sol hace que las células normales de la piel se vuelvan anormales. Estas células anormales crecen en forma rápida y descontrolada, y atacan los tejidos que están a su alrededor.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1442,131 +1442,131 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="B37" t="n">
-        <v>298915</v>
+        <v>205635</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>EN_616100_100363-10</t>
+          <t>EN_193549_46880-36</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>“They told me they bow down to a photo of Doug almost every day to thank God that he was sent to take care of their son and to improve their lives,” says Dr. Shukla.</t>
+          <t>The use of focus groups involves some limitations. First, individual dynamics may vary in a group setting and affect whether a parent contributes to the discussion or relates experiences. The overall tone and collective opinion of the group may vary from group to group, depending on the individual participants in the group.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="B38" t="n">
-        <v>264558</v>
+        <v>890615</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ES_253434_39705-1</t>
+          <t>ES_766385_101470-34</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>¿Qué es el trastorno por consumo de alcohol: El trastorno por consumo de alcohol implica tener hábitos no saludables o peligrosos de consumo de bebidas alcohólicas, como beber todos los días o beber demasiado de una sola vez. Puede variar de leve a grave. Cuantas más señales tenga, más grave puede ser el trastorno. El trastorno por consumo de alcohol de moderado a grave a veces se llama adicción.</t>
+          <t>El equipo de trasplante de médula ósea: El grupo de especialistas involucrados en el cuidado de los niños que se someten a un procedimiento de trasplante suele denominarse "equipo de trasplante", y todos sus miembros trabajan en forma conjunta para maximizar las probabilidades de un trasplante exitoso. El equipo de trasplante de médula ósea está compuesto por:</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[1, 1, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="B39" t="n">
-        <v>225076</v>
+        <v>379151</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>EN_746845_113313-49</t>
+          <t>ES_142091_35656-7</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>After aortic dissection, you can expect to be in the hospital for about a week. However, if you have complications, it could be three or four weeks.</t>
+          <t>Este evaluador identifica maneras de mejorar la gobernanza del programa y crear capacidad de liderazgo. El formulario adjunto certifica que los programas realizaron la evaluación requerida.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="B40" t="n">
-        <v>831458</v>
+        <v>113318</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>EN_299725_53465-554</t>
+          <t>ES_656398_94155-2</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15. US Department of Labor, Occupational Safety and Health Administration. 29 CFR 1910.1200. Hazard communication. Federal Register 1994;59:17479.</t>
+          <t>Si decides continuar con tu embarazo, te daremos una lista de recursos para ayudarte a obtener atención prenatal.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B41" t="n">
-        <v>351890</v>
+        <v>633502</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ES_27084_10729-3</t>
+          <t>ES_1035472_8969-54</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>El verbo principal está compuesto por la raíz y el morfema aspectual, que va sufijado al lexema y marca el aspecto perfectivo (-tu, -i, o -n), el imperfectivo (-t(z)en) y el futuro (-ko, -go, -en) (5) (6) (7).</t>
+          <t>El punto de partida de la teoría democrático-funcional de los derechos fundamentales es la concepción de los derechos fundamentales desde su función pública y política, es decir, los derechos fundamentales alcanzan su sentido y su principal significado como factores constitutivos de un libre proceso de producción democrática del Estado y de un proceso democrático de formación de la voluntad política.52 Asimismo, entre sus consecuencias destaca:\n- 1.\n- 2..</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1582,19 +1582,19 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>124620</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ES_953747_124620-3</t>
+          <t>ES_938940_123623-2</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Causas: La parte interna del oído contiene células pilosas diminutas (terminaciones nerviosas), las cuales transforman los sonidos en señales eléctricas. Los nervios llevan luego estas señales al cerebro.</t>
+          <t>Usted debe haber recibido fisioterapia mientras estuvo en el hospital o en un centro de rehabilitación antes de salir del hospital para ir a casa.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1610,19 +1610,19 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="B43" t="n">
-        <v>271594</v>
+        <v>436886</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ES_418922_52014-2</t>
+          <t>EN_1279254_283915-22</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Mostrando 1-5 de 5 médicos disponibles Inicial del apellido: M Harmeet Malhi, M.B.B.S. Hepatólogo del trasplante Rochester, MN Áreas de especialización: Colonoscopía, Endoscopia, esteatohepatitis no alcohólica, Lesión al hígado Shennen A. Mao, M.D. cirujano especializado en trasplantes Jacksonville, FL Áreas de especialización: Trasplante de hígado, Trasplante de riñón, Trasplante de páncreas Amit K. Mathur, M.D. cirujano general Phoenix, AZ Áreas de especialización: Trasplante de hígado, Trasplante de riñón, Trasplante con donante vivo, Trasplante de páncreas, Cáncer de páncreas, Cán...cer del conducto biliar, Cáncer de hígado, Cáncer de vesícula biliar Mostrar más áreas de especialización para Amit K. Mathur, M.D.</t>
+          <t>What other information should I know: Keep all appointments with your doctor and the laboratory. Your doctor may order certain lab tests to check your body's response to rivaroxaban.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1638,103 +1638,103 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="B44" t="n">
-        <v>371557</v>
+        <v>63553</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>EN_444164_64660-28</t>
+          <t>ES_422571_53403-1</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Gautier V, Chanez P, Vendrell JP, et al. Unexplained CD4-positive T-cell deficiency in non-HIV patients presenting as a Pneumocystis carinii pneumonia. Clin Exp Allergy 1991;21:63-6.</t>
+          <t>W W No hay ninguna afección que comience con la letra X X No hay ninguna afección que comience con la letra Y Y No hay ninguna afección que comience con la letra Z Z ES-View All ES-View All ES-View All Apendicitis Appendix diseases Arañas vasculares Solicite una consulta Análisis y procedimientosMédicos Jan. 27, 2024 Comparte en: FacebookTwitter Trauma, Critical Care and General Surgery in RochesterSeccionesPanorama generalAnálisis y procedimientosEnfermedades tratadasMédicosCentros, viajes y alojamientoEnsayos clínicosInvestigaciónCostos y seguroSolicita una consultaRemisiones SeccionesSolicita una consultaPanorama generalCentros, viajes y alojamientoInvestigaciónCostos y seguro ORG-20557386 Centros y departamentos médicos Trauma, Critical Care and General Surgery in Rochester</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B45" t="n">
-        <v>785498</v>
+        <v>298915</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>EN_740978_112757-6</t>
+          <t>EN_616100_100363-10</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Statistics show that there were 7,860 tuberculosis cases reported in the U.S. in 2021. The national incidence rate is 2.4 cases per 100,000 people.</t>
+          <t>“They told me they bow down to a photo of Doug almost every day to thank God that he was sent to take care of their son and to improve their lives,” says Dr. Shukla.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="B46" t="n">
-        <v>546534</v>
+        <v>940790</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>EN_526766_87197-20</t>
+          <t>EN_1334120_23665-14</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>In 2022, she reached out to the CHOP Foundation team and donated to a fund that helps cover the costs of travel for families in need of care at the CFDT. With that gift, her childhood dream has come true, and she’s helped fulfill the hopes and dreams of countless families.</t>
+          <t>Excessive noise from equipment such as chain saws, backhoes, tractors, pavement breakers, blowers, and dryers may cause ringing in the ears and subsequent hearing damage. If working with any noise that you must shout over to be heard, you should wear earplugs or other hearing protection devices.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[1, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1]</t>
+          <t>[1, 0, 0, 0]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="B47" t="n">
-        <v>369861</v>
+        <v>907379</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>EN_1263569_282171-15</t>
+          <t>EN_868259_123878-4</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Certain types of foods may worsen diarrhea and gas symptoms. This problem may be more severe during times of active disease. Diet suggestions include:\n- Eat small amounts of food throughout the day.\n- Drink plenty of water (drink small amounts throughout the day).\n- Avoid high-fiber foods (bran, beans, nuts, seeds, and popcorn).\n- Avoid fatty, greasy or fried foods and sauces (butter, margarine, and heavy cream).\n- Limit milk products if you are lactose intolerant. Dairy products are a good source of protein and calcium..</t>
+          <t>A cardiologist will review your records and decide an appropriate testing for you. After recommendations are made you will be sent to our scheduling office to get your appointments set up. The evaluation by the heart failure cardiologist may take place in the hospital or in the outpatient clinic.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1750,19 +1750,19 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="B48" t="n">
-        <v>959602</v>
+        <v>913595</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ES_776075_101950-81</t>
+          <t>ES_425882_53735-10</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>\n- El nombre de la prueba o del procedimiento\n- Los motivos por los que se realiza la prueba o el procedimiento\n- Los resultados que puede esperar y qué significan\n- Los riesgos y los beneficios de la prueba o del procedimiento\n- Los efectos secundarios y las complicaciones posibles\n- Cuándo y dónde le realizarán la prueba o el procedimiento\n- Quién es la persona que realizará la prueba o el procedimiento, y sus conocimientos o experiencia\n- Qué sucedería si no se realizara la prueba o el procedimiento\n- Las pruebas o los procedimientos alternativos disponibles\n- Cuándo y cómo obtendrá los resultados\n- A quién llamar luego de la prueba o del procedimiento en caso de tener preguntas o problemas\n- Cuánto deberá pagar por la prueba o el procedimiento</t>
+          <t>Para reducir el grosor de las uñas, debes aplicarte una loción de venta libre que contenga urea. O bien, el proveedor de atención médica puede reducir el grosor de la superficie de la uña (desbridamiento) con una lima u otra herramienta.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1778,47 +1778,47 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="B49" t="n">
-        <v>824632</v>
+        <v>621502</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>EN_729813_111974-12</t>
+          <t>ES_167903_1634-11</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>What organization actually manages the distribution of organs? What is the process to receive an organ or tissue: UNOS maintains the national Organ Procurement and Transplantation Network (OPTN). Through the UNOS Organ Center, organ donors are matched to waiting recipients 24 hours a day, 365 days a year.</t>
+          <t>Después, una vez que haya elegido a alguien que parezca adecuado o lo haya reducido a un par de opciones, también puede considerar la primera sesión o dos como una especie de prueba. También puede ser abierto con los proveedores sobre esto. Por ejemplo, podría decir: “Estamos considerando algunas opciones en este momento, pero nos gustaría tener una primera sesión con usted y ver cómo funciona”. Los proveedores son profesionales, ellos entienden lo importante que es que haya un buen ajuste y no lo tomarán personalmente si decide ir en otra dirección. Muchos proveedores también ofrecen consultas telefónicas gratuitas, que pueden ser una forma útil para que usted y su hijo tengan una mejor idea de cómo sería trabajar con ellos.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 1]</t>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="B50" t="n">
-        <v>400572</v>
+        <v>59738</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ES_508330_6525-223</t>
+          <t>ES_448604_59723-1</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>GLNPO: (Great Lakes National Program Office). Oficina del Programa Nacional de los Grandes Lagos</t>
+          <t>W W No hay ningún médico cuyo apellido comience con dicha letra X X Buscar un médico cuyo apellido comience con una letra Y Y Buscar un médico cuyo apellido comience con una letra Z Z Ver todo By Location: View All Rochester, MN Mauro H. Schenone, M.D. Rochester, MN Área de especialización: Ecografía fetal, Muestreo de vellosidades coriónicas, Cirugía fetal, ablación láser fetoscópica, ablación por radiofrecuencia, cirugía para liberación de bandas amnióticas, transfusión intrauterina, fetoscopía, colocación de derivación para feto, Muestra sanguínea umbilical percutánea, Procedimiento EXIT (tratamiento extrauterino intraparto), hernia diafragmática congénita, anemia fetal, enfermedad cardíaca fetal, Gemelos unidos, mielomeningocele, teratoma sacrococcígeo, secuencia TRAP, síndrome congénito de obstrucción de vías respiratorias superiores, síndrome de banda amniótica, Cardiopatía congénita, malformación quística adenomatosa congénita, efusión pleural, síndrome de la transfusión de mellizo a mellizo, Hidropesía fetal, doble secuencia anemia-policitemia, obstrucción de la salida de la vejiga, Isoinmunización fetal Chandra C. Shenoy, M.D. Rochester, MN Área de especialización: Donación de óvulos, Congelación de óvulos, Inseminación intrauterina, Fertilización in vitro, polipectomía, Donación de esperma, Histeroscopia, Preservación de la fertilidad, Histerosalpingografía, asesoría genética, sustitución gestacional, pruebas genéticas preimplantatorias, congelación de esperma, Cirugía de reducción de masa, imágenes tridimensionales, Inyección de esperma intracitoplasmático, Transferencia de embriones, Inducción de la ovulación, congelamiento de embriones, Pólipos uterinos, Amenorrea sin otra indicación, Hipotiroidismo, Síndrome de ovario poliquístico, Infertilidad, insuficiencia ovárica primaria, Aborto espontáneo recurrente, ciclo menstrual irregular, Trastornos del ciclo menstrual, Hiperprolactinemia, Maternidad en edad avanzada Viji Shridhar, Ph.D. Rochester, MN Área de especialización: Cáncer, Tumores y masas Ebbie A. Stewart, M.D. Rochester, MN Área de especialización: Donación de óvulos, Cirugía focalizada por ultrasonido , Congelación de óvulos, Cirugía mínimamente invasiva, Inseminación intrauterina, Fertilización in vitro, Miomectomía, polipectomía, Tecnología de reproducción asistida, Preservación de la fertilidad, Histerosalpingografía, pruebas genéticas preimplantatorias, histeroscopía diagnóstica, Laparoscopía diagnóstica, Cirugía ginecológica, Transferencia de embriones, Inducción de la ovulación, congelamiento de embriones, Sangrado menstrual abundante, Pólipos uterinos, Fibromas uterinos, Amenorrea sin otra indicación, Hipotiroidismo, Infertilidad, insuficiencia ovárica primaria, Adenomiosis, Útero doble, Aborto espontáneo recurrente, útero tabicado, anomalía uterina, ciclo menstrual irregular, Hiperprolactinemia Linda M. Szymanski, M.D., Ph.D. Rochester, MN Profesionales médicos Obstetrics &amp; Gynecology physicians</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1834,29 +1834,393 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="B51" t="n">
-        <v>940743</v>
+        <v>663186</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>EN_1248507_281011-5</t>
+          <t>EN_311588_53676-206</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Antibodies may be produced when your immune system mistakenly considers healthy tissue to be a harmful substance. In the case of platelet antibodies, your body created antibodies to attack platelets. As a result, you will have a lower than normal number of platelets in your body. This condition is called thrombocytopenia, and it can cause too much bleeding.</t>
+          <t>The sponsor should ensure that the designated PHS specimens from the source animals, xenotransplantation products, and xenotransplantation product recipients are archived (sections 3.7.1, 3.5.3, and 4.1.2.). The biologic specimens should be collected and archived under conditions that will ensure their suitability for subsequent public health purposes, including public health investigations (sections 4.1.2.3.). The location and nature of archived specimens should be documented in the health care records and this information should be linked to the National Xenotransplantation Database when the latter becomes functional.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B52" t="n">
+        <v>520497</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ES_272255_40278-55</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Cirugía en niños: En la mayoría de los casos, un niño con una hernia inguinal necesitará cirugía para corregirla.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[1, 1, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[1, 1, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B53" t="n">
+        <v>824655</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>EN_787651_117039-3</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Most people with mechanical back pain experience pain primarily in their lower back. The pain may radiate (spread) to your buttocks and thighs. Many people may also experience spasms with mechanical back pain. The symptoms of mechanical back pain are generally more noticeable with flexion of the back and when lifting heavy objects.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B54" t="n">
+        <v>239279</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ES_1029178_131258-4</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>(3.5 x 2 pulg.)\n- Bloques de papel para proveedores médicos. Cada bloque incluye 25 hojas que se les pueden dar a pacientes interesados en los estudios observacionales de embarazo de MotherToBaby. Bloques de papel específicos disponibles para las especialidades de Alergólogos e Inmunólogos, Dermatólogos, Gastroenterólogos, Neurólogos, y Reumatólogos. (3.5 x 5pulg.)\n- Un volante para pacientes que contesta preguntas comunes y explica el proceso de participar en los estudios de embarazo observacionales de MotherToBaby. Disponible en inglés y español y empaquetado en cantidades de 50. Por favor indique el número total que desea. (8.5 x 11 pulg.)\n- Una tarjeta informativa sobre si bombear y desechar la leche de pecho es necesario cuando se toma medicamento. Incluye maneras de contactar al servicio de información gratuito de MotherToBaby California. (5.5 x 4.25 pulg.)</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1053367</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ES_349351_42861-13</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>¿Cómo se diagnostican las aftas: Las aftas son bastante frecuentes, pero eso no significa que se deban ignorar. Si tienes aftas que te duran más de dos semanas o no puedes comer o beber por el dolor que te provocan, llama a tu médico. Llámalo también si tienes aftas más de dos o tres veces al año.</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B56" t="n">
+        <v>577384</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>EN_766456_115024-30</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Reviewed on Aug 25, 2022: Very good experience from making the appointment to seeing the doctor and scheduling additional appointments at front desk. Hardly any waiting time to see the doctor and her assistant. Both the doctor's assistant and Dr. Anaim Baig from the Neurology Dept were very cordial and efficient, I felt very well attended to as all my concerns were addressed. Great team!</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B57" t="n">
+        <v>946354</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>EN_168698_4069-8</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Scorpio: You’re going through some big changes right now. And some of those changes may involve your dating life. You may be finding yourself drawn to love interests who are pretty different from who you’ve gone for in the past. (Big age difference? Weird job? Super interesting aesthetic?) But that doesn’t mean that they’re not going to be a great match for you. In fact, this month may be an especially emotionally connected month for you when it comes to dating. Knowing you, that means beginning to invest your heart deeply. If things feel solid between you and your love interest by the end of the month, then this relationship is likely to have a future.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ES_490955_64059-16</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Cada vez está más claro, en especial en el caso de los meduloblastomas, que el desenlace también se relaciona con las características moleculares del tumor; sin embargo, esto no se ha demostrado de forma definitiva en el caso de otros tumores embrionarios.[1,5,6,19-21] Las tasas de SG oscilan entre el 40 % y el 90 %, según el subtipo molecular de meduloblastoma y, posiblemente, según otros factores como el grado de diseminación en el momento del diagnóstico y el alcance de la resección. Los niños con meduloblastoma que sobreviven durante 5 años se consideran curados de su tumor. Por lo general, las tasas de supervivencia para otros tumores son más precarias y oscilan entre el 5 % y el 50 %. Las tasas de supervivencia específicas se tratan en cada subgrupo en este resumen.[22-25]</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[1, 1, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>[1, 1, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" t="n">
+        <v>795769</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>EN_1325459_22447-2</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>If you develop a sudden hearing loss, contact your doctor immediately. Some treatments may help minimize the damage and reduce the severity of the hearing loss.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B60" t="n">
+        <v>485943</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>EN_723876_111631-4</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>From your lungs, your bloodstream delivers oxygen to all your organs and other tissues.</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B61" t="n">
+        <v>785502</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>EN_567629_92967-10</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Immunoglobulin treatments: In certain situations, antibodies obtained from animals, from other people, or synthesized in a laboratory can be used to treat individuals at risk of infections. For example, infants born to women infected with hepatitis B are treated with antibody preparations in addition to being vaccinated in an effort to protect them from also becoming infected with hepatitis B. In another example, people bitten by some poisonous snakes may be treated with antivenom, a mixture of antibodies against the type of snake venom to which the person was exposed.</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B62" t="n">
+        <v>265186</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>EN_1290105_286287-2</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Polycystin-1 is also found in cell structures called primary cilia. Primary cilia are tiny, fingerlike projections that line the small tubes where urine is formed (renal tubules). Researchers believe that primary cilia sense the movement of fluid through these tubules, which appears to help maintain the tubules' size and structure. The interaction of polycystin-1 and polycystin-2 in renal tubules promotes the normal development and function of the kidneys.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B63" t="n">
+        <v>785514</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>EN_1271923_283144-9</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Opicapone may cause other side effects. Call your doctor if you have any unusual problems while taking this medication.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B64" t="n">
+        <v>92735</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>EN_991397_17534-0</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Marijuana: Using marijuana while breastfeeding can allow harmful chemicals to pass from the mother to the infant through breast milk or secondhand smoke exposure. To limit potential risk to the infant, breastfeeding mothers should be advised not to use marijuana or products containing cannabidiol (CBD) in any form while breastfeeding.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 0]</t>
         </is>
       </c>
     </row>

</xml_diff>